<commit_message>
reorder,organize and add sample msa script
</commit_message>
<xml_diff>
--- a/data/Table_S1B_final.xlsx
+++ b/data/Table_S1B_final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steveabecassis/Desktop/Thesis/Papers Thesis/data/AlphaFold2 fails to predict protein fold switching/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steveabecassis/PycharmProjects/MsaCluster/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F16BE27-B515-2949-B978-34BC9AE93BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F874100-3A18-6845-8A0F-1710F72619A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36220" yWindow="500" windowWidth="31480" windowHeight="21100" xr2:uid="{877DB3DD-AC65-0347-87C1-56B11B34E303}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20660" xr2:uid="{877DB3DD-AC65-0347-87C1-56B11B34E303}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -681,12 +681,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -701,7 +707,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -717,6 +723,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1041,20 +1053,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D599E226-3A67-7D44-AB5A-E6C30942311B}">
-  <dimension ref="A1:G94"/>
+  <dimension ref="A1:H94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G89" sqref="A89:G89"/>
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.83203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
@@ -1426,7 +1438,7 @@
         <v>47.5</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>22</v>
       </c>
@@ -1449,7 +1461,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
@@ -1472,7 +1484,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>26</v>
       </c>
@@ -1495,7 +1507,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>28</v>
       </c>
@@ -1518,7 +1530,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>128</v>
       </c>
@@ -1541,7 +1553,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>118</v>
       </c>
@@ -1564,7 +1576,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>30</v>
       </c>
@@ -1587,7 +1599,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>116</v>
       </c>
@@ -1610,7 +1622,7 @@
         <v>99.7</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>114</v>
       </c>
@@ -1633,7 +1645,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>32</v>
       </c>
@@ -1656,7 +1668,7 @@
         <v>95.7</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>112</v>
       </c>
@@ -1679,7 +1691,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>182</v>
       </c>
@@ -1702,7 +1714,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>130</v>
       </c>
@@ -1725,7 +1737,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>110</v>
       </c>
@@ -1748,7 +1760,7 @@
         <v>71.400000000000006</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>124</v>
       </c>
@@ -1771,27 +1783,30 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32" s="8">
         <v>0.39</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32" s="8">
         <v>16.170000000000002</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32" s="7">
         <v>0.3</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F32" s="8">
         <v>15.73</v>
       </c>
-      <c r="G32" s="1">
-        <v>100</v>
+      <c r="G32" s="8">
+        <v>100</v>
+      </c>
+      <c r="H32" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
try to fix support path
</commit_message>
<xml_diff>
--- a/data/Table_S1B_final.xlsx
+++ b/data/Table_S1B_final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steveabecassis/PycharmProjects/MsaCluster/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F874100-3A18-6845-8A0F-1710F72619A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF1EE60-F2A2-2947-AC55-AB4975B5BE99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20660" xr2:uid="{877DB3DD-AC65-0347-87C1-56B11B34E303}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20680" xr2:uid="{877DB3DD-AC65-0347-87C1-56B11B34E303}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -695,7 +695,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -703,11 +703,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -725,10 +740,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -749,11 +770,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="pdbids_str_seq_comparisons" connectionId="2" xr16:uid="{15383BDE-0473-D04A-A4F4-C271CC7E7B22}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="pdbids_rmsds" connectionId="1" xr16:uid="{CDDF0B48-A0E1-CE4B-A361-4C4D4B85A73A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="pdbids_rmsds" connectionId="1" xr16:uid="{CDDF0B48-A0E1-CE4B-A361-4C4D4B85A73A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="pdbids_str_seq_comparisons" connectionId="2" xr16:uid="{15383BDE-0473-D04A-A4F4-C271CC7E7B22}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1056,7 +1077,7 @@
   <dimension ref="A1:H94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -1065,8 +1086,8 @@
     <col min="3" max="3" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" style="2" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" style="2" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
@@ -1140,48 +1161,48 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="8">
         <v>0.23</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="8">
         <v>7.26</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="7">
         <v>0.09</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="8">
         <v>5.63</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="8">
         <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="8">
         <v>0.28999999999999998</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="8">
         <v>20.43</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="7">
         <v>0.17</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="8">
         <v>3.16</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="8">
         <v>100</v>
       </c>
     </row>
@@ -1784,25 +1805,25 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="C32" s="8">
+      <c r="C32" s="10">
         <v>0.39</v>
       </c>
-      <c r="D32" s="8">
+      <c r="D32" s="10">
         <v>16.170000000000002</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="9">
         <v>0.3</v>
       </c>
-      <c r="F32" s="8">
+      <c r="F32" s="10">
         <v>15.73</v>
       </c>
-      <c r="G32" s="8">
+      <c r="G32" s="10">
         <v>100</v>
       </c>
       <c r="H32" s="2">

</xml_diff>